<commit_message>
N-S Abutments, 7_wy2016-2019, pTHg:  Replaced 7_pTHg model results file; Added Sigma Plot folder; Replaced N Abutment pTHg folder; Replaced S Abutment pTHg folder; Updated S Abutment Q+WQ worksheet; Updated N Abutment Q+WQ worksheet; Updated Loads Progress worksheet.
</commit_message>
<xml_diff>
--- a/2018-19_CCSB_LoadsData_WY2010-2018/Sites/S_Abutment_11452800/7_wy2016-19/7_rloadest/7_pTHg/7_Excel for Text Files/pTHg_SWeirR.xlsx
+++ b/2018-19_CCSB_LoadsData_WY2010-2018/Sites/S_Abutment_11452800/7_wy2016-19/7_rloadest/7_pTHg/7_Excel for Text Files/pTHg_SWeirR.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018-19_CCSB_LoadsData_WY2010-2018\Sites\S_Abutment_11452800\7_wy2016-19\7_pTHg\7_Excel for Text Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018-19_CCSB_LoadsData_WY2010-2018\Sites\S_Abutment_11452800\7_wy2016-19\7_rloadest\7_pTHg\7_Excel for Text Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31106DFE-797B-4F7A-8010-74F405A052B7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{594C159C-9766-41DC-B344-887E3AE218F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{69CA5FB9-84F0-4066-91E6-B304E311EDA6}"/>
+    <workbookView xWindow="6660" yWindow="405" windowWidth="15420" windowHeight="15630" xr2:uid="{6B42F4B4-ACBA-4C0D-AA81-3031A41FEA52}"/>
   </bookViews>
   <sheets>
-    <sheet name="6_pTHg" sheetId="1" r:id="rId1"/>
+    <sheet name="7_pTHg" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -411,7 +411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C07DBF-DDF2-4DC5-AFA5-AC009C721F20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1428DA8C-8369-413F-9B38-9654C840517C}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
@@ -842,7 +842,7 @@
         <v>0.55381944444444442</v>
       </c>
       <c r="C30" s="3">
-        <v>11138</v>
+        <v>11134</v>
       </c>
       <c r="D30">
         <v>473</v>

</xml_diff>